<commit_message>
got an early version of the velocity slow down on approach working
</commit_message>
<xml_diff>
--- a/output/hold_crush_tests.xlsx
+++ b/output/hold_crush_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattmacdonald/Gitlab/crush-rig/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7241A2D-CA27-B24B-8489-86019E1A154C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADFF2B9-E561-B748-84E1-A1ABD6CFF4CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16560" activeTab="1" xr2:uid="{55546BDD-9D33-AC48-88A7-DE9EB5A2D870}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Timestamp (s)</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Target N</t>
+  </si>
+  <si>
+    <t>N/s</t>
+  </si>
+  <si>
+    <t>force - avg_force</t>
+  </si>
+  <si>
+    <t>delta</t>
   </si>
 </sst>
 </file>
@@ -19449,6 +19458,830 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'181027-2'!$G$73</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'181027-2'!$A$74:$A$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>2.3537089999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3859319999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4179889999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.449967</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.481824</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5140159999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5459309999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5779960000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.609696</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6414979999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6738759999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.7056309999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.7380900000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.769987</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8017189999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.8341889999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.866161</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.8980250000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.929843</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.9622470000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.9940859999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.0261179999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.058109</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.0903170000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.122134</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.1540729999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2016619999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.2340960000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.2662810000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.2980580000000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.3299569999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3621439999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'181027-2'!$G$74:$G$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.85732165206508704</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.85032430251683222</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7094550332220726</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.85683907686534355</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7022862823061753</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85853047156509088</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.728706624605687</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5847430979183796</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.2312681450367515</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0399937017792515</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.7531347238053652</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.8721196350754346</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.6348165889323401</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5947028025870083</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.5699987489052631</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.318855134320826</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.194921113834965</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.992470065423984</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12.908696881183566</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.830919080919058</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17.129817761245295</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19.566567312468816</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.696420152748736</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>31.741757725664602</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>29.363928638971267</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23.654190047480817</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-3.4053130340220576</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.8589610959591325</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.85127535961724055</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-7FB7-844A-8046-59A5EB6544DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1639867503"/>
+        <c:axId val="1639140175"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'181027-2'!$H$73</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>force - avg_force</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'181027-2'!$A$74:$A$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>2.3537089999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3859319999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4179889999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.449967</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.481824</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5140159999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5459309999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5779960000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.609696</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6414979999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6738759999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.7056309999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.7380900000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.769987</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8017189999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.8341889999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.866161</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.8980250000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.929843</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.9622470000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.9940859999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.0261179999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.058109</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.0903170000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.122134</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.1540729999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2016619999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.2340960000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.2662810000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.2980580000000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.3299569999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3621439999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'181027-2'!$H$74:$H$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.369999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.369999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.739999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.3700000000000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7400000000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3700000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7400000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1100000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.8500000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.5899999999999985E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.10960000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.10960000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.13700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.12330000000000019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.13700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1644000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.17810000000000015</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.1780999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.20550000000000024</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.20549999999999979</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.27400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.31510000000000016</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.42469999999999963</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.50689999999999991</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.69869999999999965</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.3835999999999995</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-5.4800000000000182E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.3700000000000045E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.3700000000000045E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-7FB7-844A-8046-59A5EB6544DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1643308031"/>
+        <c:axId val="1643305023"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1639867503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1639140175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1639140175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1639867503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1643305023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1643308031"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1643308031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1643305023"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -19490,6 +20323,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -20561,6 +21434,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -20637,6 +22026,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6BA972A-6A46-E34D-9453-42E95565339D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -31281,10 +32706,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A8530A-99F0-904E-8F82-557DF0E4C7D3}">
-  <dimension ref="A1:H513"/>
+  <dimension ref="A1:I513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="N91" sqref="N91"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="I88" sqref="H88:I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -31363,6 +32788,10 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="H3">
+        <f>0.01*H2</f>
+        <v>5.8860000000000003E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
@@ -32584,7 +34013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:9">
       <c r="A65">
         <v>2.0656880000000002</v>
       </c>
@@ -32604,7 +34033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:9">
       <c r="A66">
         <v>2.0976089999999998</v>
       </c>
@@ -32624,7 +34053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:9">
       <c r="A67">
         <v>2.1296789999999999</v>
       </c>
@@ -32644,7 +34073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:9">
       <c r="A68">
         <v>2.161235</v>
       </c>
@@ -32664,7 +34093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:9">
       <c r="A69">
         <v>2.193454</v>
       </c>
@@ -32684,7 +34113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:9">
       <c r="A70">
         <v>2.2254870000000002</v>
       </c>
@@ -32704,7 +34133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:9">
       <c r="A71">
         <v>2.2577129999999999</v>
       </c>
@@ -32724,7 +34153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:9">
       <c r="A72">
         <v>2.289901</v>
       </c>
@@ -32744,7 +34173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:9">
       <c r="A73">
         <v>2.3217490000000001</v>
       </c>
@@ -32763,8 +34192,17 @@
       <c r="F73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74">
         <v>2.3537089999999998</v>
       </c>
@@ -32783,8 +34221,20 @@
       <c r="F74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74">
+        <f t="shared" ref="G74:G79" si="0">(D74-D73)/(A74-A73)</f>
+        <v>0.85732165206508704</v>
+      </c>
+      <c r="H74">
+        <f>D74 - AVERAGE(D73:D74)</f>
+        <v>1.369999999999999E-2</v>
+      </c>
+      <c r="I74">
+        <f>D74-D73</f>
+        <v>2.739999999999998E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75">
         <v>2.3859319999999999</v>
       </c>
@@ -32803,8 +34253,20 @@
       <c r="F75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75">
+        <f t="shared" si="0"/>
+        <v>-0.85032430251683222</v>
+      </c>
+      <c r="H75">
+        <f t="shared" ref="H75:H101" si="1">D75 - AVERAGE(D74:D75)</f>
+        <v>-1.369999999999999E-2</v>
+      </c>
+      <c r="I75">
+        <f t="shared" ref="I75:I105" si="2">D75-D74</f>
+        <v>-2.739999999999998E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76">
         <v>2.4179889999999999</v>
       </c>
@@ -32823,8 +34285,20 @@
       <c r="F76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76">
+        <f t="shared" si="0"/>
+        <v>1.7094550332220726</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="1"/>
+        <v>2.739999999999998E-2</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="2"/>
+        <v>5.4799999999999988E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77">
         <v>2.449967</v>
       </c>
@@ -32843,8 +34317,20 @@
       <c r="F77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77">
+        <f t="shared" si="0"/>
+        <v>-0.85683907686534355</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="1"/>
+        <v>-1.3700000000000018E-2</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="2"/>
+        <v>-2.7400000000000008E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78">
         <v>2.481824</v>
       </c>
@@ -32863,8 +34349,20 @@
       <c r="F78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79">
         <v>2.5140159999999998</v>
       </c>
@@ -32883,8 +34381,20 @@
       <c r="F79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <f t="shared" si="0"/>
+        <v>1.7022862823061753</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="1"/>
+        <v>2.7400000000000008E-2</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="2"/>
+        <v>5.4800000000000015E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80">
         <v>2.5459309999999999</v>
       </c>
@@ -32903,8 +34413,20 @@
       <c r="F80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <f>(D80-D79)/(A80-A79)</f>
+        <v>0.85853047156509088</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="1"/>
+        <v>1.3700000000000004E-2</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="2"/>
+        <v>2.7399999999999994E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81">
         <v>2.5779960000000002</v>
       </c>
@@ -32923,8 +34445,20 @@
       <c r="F81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <f t="shared" ref="G81:G101" si="3">(D81-D80)/(A81-A80)</f>
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82">
         <v>2.609696</v>
       </c>
@@ -32943,8 +34477,20 @@
       <c r="F82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82">
+        <f t="shared" si="3"/>
+        <v>1.728706624605687</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="1"/>
+        <v>2.7400000000000004E-2</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="2"/>
+        <v>5.4800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83">
         <v>2.6414979999999999</v>
       </c>
@@ -32963,8 +34509,20 @@
       <c r="F83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83">
+        <f t="shared" si="3"/>
+        <v>2.5847430979183796</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="1"/>
+        <v>4.1100000000000005E-2</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="2"/>
+        <v>8.2200000000000009E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84">
         <v>2.6738759999999999</v>
       </c>
@@ -32983,8 +34541,20 @@
       <c r="F84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84">
+        <f t="shared" si="3"/>
+        <v>4.2312681450367515</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="1"/>
+        <v>6.8500000000000005E-2</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="2"/>
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85">
         <v>2.7056309999999999</v>
       </c>
@@ -33003,8 +34573,20 @@
       <c r="F85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85">
+        <f t="shared" si="3"/>
+        <v>6.0399937017792515</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="1"/>
+        <v>9.5899999999999985E-2</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="2"/>
+        <v>0.1918</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86">
         <v>2.7380900000000001</v>
       </c>
@@ -33023,8 +34605,20 @@
       <c r="F86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="G86">
+        <f t="shared" si="3"/>
+        <v>6.7531347238053652</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="1"/>
+        <v>0.10960000000000003</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="2"/>
+        <v>0.21919999999999995</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87">
         <v>2.769987</v>
       </c>
@@ -33043,8 +34637,20 @@
       <c r="F87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="G87">
+        <f t="shared" si="3"/>
+        <v>6.8721196350754346</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="1"/>
+        <v>0.10960000000000003</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="2"/>
+        <v>0.21920000000000006</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88">
         <v>2.8017189999999998</v>
       </c>
@@ -33063,8 +34669,20 @@
       <c r="F88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="G88">
+        <f t="shared" si="3"/>
+        <v>8.6348165889323401</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="2"/>
+        <v>0.27399999999999991</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89">
         <v>2.8341889999999998</v>
       </c>
@@ -33083,8 +34701,20 @@
       <c r="F89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="G89">
+        <f t="shared" si="3"/>
+        <v>7.5947028025870083</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="1"/>
+        <v>0.12330000000000019</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="2"/>
+        <v>0.24660000000000015</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90">
         <v>2.866161</v>
       </c>
@@ -33103,8 +34733,20 @@
       <c r="F90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="G90">
+        <f t="shared" si="3"/>
+        <v>8.5699987489052631</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="1"/>
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="2"/>
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91">
         <v>2.8980250000000001</v>
       </c>
@@ -33123,8 +34765,20 @@
       <c r="F91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="G91">
+        <f t="shared" si="3"/>
+        <v>10.318855134320826</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="1"/>
+        <v>0.1644000000000001</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="2"/>
+        <v>0.32879999999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92">
         <v>2.929843</v>
       </c>
@@ -33143,8 +34797,20 @@
       <c r="F92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="G92">
+        <f t="shared" si="3"/>
+        <v>11.194921113834965</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="1"/>
+        <v>0.17810000000000015</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="2"/>
+        <v>0.35619999999999985</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93">
         <v>2.9622470000000001</v>
       </c>
@@ -33163,8 +34829,20 @@
       <c r="F93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="G93">
+        <f t="shared" si="3"/>
+        <v>10.992470065423984</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="1"/>
+        <v>0.1780999999999997</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="2"/>
+        <v>0.35619999999999985</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94">
         <v>2.9940859999999998</v>
       </c>
@@ -33183,8 +34861,20 @@
       <c r="F94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="G94">
+        <f t="shared" si="3"/>
+        <v>12.908696881183566</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="1"/>
+        <v>0.20550000000000024</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="2"/>
+        <v>0.41100000000000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95">
         <v>3.0261179999999999</v>
       </c>
@@ -33203,8 +34893,20 @@
       <c r="F95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="G95">
+        <f t="shared" si="3"/>
+        <v>12.830919080919058</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="1"/>
+        <v>0.20549999999999979</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="2"/>
+        <v>0.41100000000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96">
         <v>3.058109</v>
       </c>
@@ -33223,8 +34925,20 @@
       <c r="F96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="G96">
+        <f t="shared" si="3"/>
+        <v>17.129817761245295</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="1"/>
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="2"/>
+        <v>0.54800000000000004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97">
         <v>3.0903170000000002</v>
       </c>
@@ -33243,8 +34957,20 @@
       <c r="F97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="G97">
+        <f t="shared" si="3"/>
+        <v>19.566567312468816</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="1"/>
+        <v>0.31510000000000016</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="2"/>
+        <v>0.63020000000000032</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98">
         <v>3.122134</v>
       </c>
@@ -33263,8 +34989,20 @@
       <c r="F98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="G98">
+        <f t="shared" si="3"/>
+        <v>26.696420152748736</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="1"/>
+        <v>0.42469999999999963</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="2"/>
+        <v>0.84940000000000015</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
       <c r="A99">
         <v>3.1540729999999999</v>
       </c>
@@ -33283,8 +35021,20 @@
       <c r="F99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="G99">
+        <f t="shared" si="3"/>
+        <v>31.741757725664602</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="1"/>
+        <v>0.50689999999999991</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="2"/>
+        <v>1.0137999999999998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100">
         <v>3.2016619999999998</v>
       </c>
@@ -33303,8 +35053,20 @@
       <c r="F100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100">
+        <f t="shared" si="3"/>
+        <v>29.363928638971267</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="1"/>
+        <v>0.69869999999999965</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="2"/>
+        <v>1.3974000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101">
         <v>3.2340960000000001</v>
       </c>
@@ -33323,8 +35085,20 @@
       <c r="F101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="G101">
+        <f t="shared" si="3"/>
+        <v>23.654190047480817</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="1"/>
+        <v>0.3835999999999995</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="2"/>
+        <v>0.76719999999999988</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
       <c r="A102">
         <v>3.2662810000000002</v>
       </c>
@@ -33343,8 +35117,20 @@
       <c r="F102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="G102">
+        <f t="shared" ref="G102:G105" si="4">(D102-D101)/(A102-A101)</f>
+        <v>-3.4053130340220576</v>
+      </c>
+      <c r="H102">
+        <f t="shared" ref="H102:H105" si="5">D102 - AVERAGE(D101:D102)</f>
+        <v>-5.4800000000000182E-2</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="2"/>
+        <v>-0.10960000000000036</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="A103">
         <v>3.2980580000000002</v>
       </c>
@@ -33363,8 +35149,20 @@
       <c r="F103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
       <c r="A104">
         <v>3.3299569999999998</v>
       </c>
@@ -33383,8 +35181,20 @@
       <c r="F104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="G104">
+        <f t="shared" si="4"/>
+        <v>0.8589610959591325</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="5"/>
+        <v>1.3700000000000045E-2</v>
+      </c>
+      <c r="I104">
+        <f t="shared" si="2"/>
+        <v>2.7400000000000091E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
       <c r="A105">
         <v>3.3621439999999998</v>
       </c>
@@ -33403,8 +35213,20 @@
       <c r="F105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105">
+        <f t="shared" si="4"/>
+        <v>0.85127535961724055</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="5"/>
+        <v>1.3700000000000045E-2</v>
+      </c>
+      <c r="I105">
+        <f t="shared" si="2"/>
+        <v>2.7400000000000091E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
       <c r="A106">
         <v>3.394075</v>
       </c>
@@ -33424,7 +35246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:9">
       <c r="A107">
         <v>3.4262079999999999</v>
       </c>
@@ -33444,7 +35266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:9">
       <c r="A108">
         <v>3.4581379999999999</v>
       </c>
@@ -33464,7 +35286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:9">
       <c r="A109">
         <v>3.4901490000000002</v>
       </c>
@@ -33484,7 +35306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:9">
       <c r="A110">
         <v>3.5220850000000001</v>
       </c>
@@ -33504,7 +35326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:9">
       <c r="A111">
         <v>3.5541640000000001</v>
       </c>
@@ -33524,7 +35346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:9">
       <c r="A112">
         <v>3.5862090000000002</v>
       </c>

</xml_diff>